<commit_message>
v0.2.2.5. Check whether a marker reference is correct
</commit_message>
<xml_diff>
--- a/templates/MC-21.xlsx
+++ b/templates/MC-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Projects\ResponseAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF3C611-B88C-4F83-B2E6-4EBC41C0323A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BC2DA1-3EFA-4A61-BB39-6AB38FC29605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
   </bookViews>
@@ -444,8 +444,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.6769532003387787"/>
           <c:y val="0.5654300373257366"/>
-          <c:w val="0.1175335203217085"/>
-          <c:h val="6.5438382968994804E-2"/>
+          <c:w val="0.11810066133620897"/>
+          <c:h val="6.4928271866372581E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1794,8 +1794,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.66361797228279218"/>
           <c:y val="0.63065121822551684"/>
-          <c:w val="0.11929117354657981"/>
-          <c:h val="6.4610747433973784E-2"/>
+          <c:w val="0.12088832699537788"/>
+          <c:h val="6.4113409016644002E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -11983,8 +11983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3406B6-B537-451D-BC5F-1BF62CD9F844}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>